<commit_message>
charts get displayed properly for both SE and TE students
</commit_message>
<xml_diff>
--- a/workbooks/registration_details.xlsx
+++ b/workbooks/registration_details.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="110" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
@@ -638,6 +638,38 @@
         </is>
       </c>
       <c r="F6" t="inlineStr">
+        <is>
+          <t>student</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>R-22-0124</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>r220124@famt.ac.in</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Mansi Surendra Agre</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>abcd@gmail.com</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>$2b$12$NH5vRBM2YWaelWJPnz.K4.gj1i5TQo3qXdUURWAKRekdm9uGxumSO</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>student</t>
         </is>

</xml_diff>

<commit_message>
atendance displayed to teacher, along with a chart for frequently absence days
</commit_message>
<xml_diff>
--- a/workbooks/registration_details.xlsx
+++ b/workbooks/registration_details.xlsx
@@ -686,7 +686,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
@@ -885,6 +885,33 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>samikb@gmail.com</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ABCD</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$2b$12$Mbu0Y4wabzc0HchfxKPOIukURdO71QwM2sHmt4U.esjDlNzJkRyi2</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>teacher</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>DSGT, DLCOA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>